<commit_message>
serial number veto feature, adding position to reporting
</commit_message>
<xml_diff>
--- a/Messages/analysis/mini_dev_results_stories_01.xlsx
+++ b/Messages/analysis/mini_dev_results_stories_01.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="254">
   <si>
     <t>Group ID</t>
   </si>
@@ -780,6 +780,15 @@
   </si>
   <si>
     <t>story count</t>
+  </si>
+  <si>
+    <t>&lt;resolved&gt; all others in group are standalone</t>
+  </si>
+  <si>
+    <t>&lt;resolved&gt; group context length</t>
+  </si>
+  <si>
+    <t>&lt;resolved&gt; last token is emoji</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1272,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1272,7 +1281,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1594,11 +1602,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A194" sqref="A192:XFD194"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="Q59" sqref="Q59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1616,7 @@
     <col min="17" max="17" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +1672,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1010</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1010</v>
       </c>
@@ -1763,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1011</v>
       </c>
@@ -1813,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1011</v>
       </c>
@@ -1863,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1011</v>
       </c>
@@ -1913,7 +1922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1011</v>
       </c>
@@ -1963,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1012</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1012</v>
       </c>
@@ -2069,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1013</v>
       </c>
@@ -2119,7 +2128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1013</v>
       </c>
@@ -2169,7 +2178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1014</v>
       </c>
@@ -2219,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1014</v>
       </c>
@@ -2269,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1015</v>
       </c>
@@ -2319,7 +2328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1015</v>
       </c>
@@ -2369,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1016</v>
       </c>
@@ -2419,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1016</v>
       </c>
@@ -2469,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -2519,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1017</v>
       </c>
@@ -2569,7 +2578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1018</v>
       </c>
@@ -2619,7 +2628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1018</v>
       </c>
@@ -2669,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1018</v>
       </c>
@@ -2719,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1019</v>
       </c>
@@ -2769,7 +2778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1019</v>
       </c>
@@ -2875,7 +2884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1020</v>
       </c>
@@ -2925,7 +2934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1020</v>
       </c>
@@ -2975,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1020</v>
       </c>
@@ -3025,7 +3034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1021</v>
       </c>
@@ -3075,119 +3084,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>1021</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>12885</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30">
         <v>32</v>
       </c>
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2">
-        <v>1</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1</v>
-      </c>
-      <c r="K30" s="2">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
         <v>9.7531152647975006</v>
       </c>
-      <c r="L30" s="2">
-        <v>1</v>
-      </c>
-      <c r="M30" s="2">
-        <v>0</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1</v>
-      </c>
-      <c r="O30" s="2">
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
         <v>2.2675675675675602</v>
       </c>
-      <c r="P30" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="R30" s="2">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>253</v>
+      </c>
+      <c r="R30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>1022</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>12888</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31">
         <v>8</v>
       </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
-      <c r="I31" s="2">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
         <v>10</v>
       </c>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
-      <c r="M31" s="2">
-        <v>0</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1</v>
-      </c>
-      <c r="O31" s="2">
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
         <v>10</v>
       </c>
-      <c r="P31" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="R31" s="2">
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>253</v>
+      </c>
+      <c r="R31">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1022</v>
       </c>
@@ -3237,63 +3246,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+    <row r="33" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>1023</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="2">
         <v>12890</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="2">
         <v>68</v>
       </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4">
-        <v>1</v>
-      </c>
-      <c r="G33" s="4">
-        <v>1</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0</v>
-      </c>
-      <c r="I33" s="4">
-        <v>0</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0</v>
-      </c>
-      <c r="K33" s="4">
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
         <v>5.4567901234567797</v>
       </c>
-      <c r="L33" s="4">
-        <v>1</v>
-      </c>
-      <c r="M33" s="4">
-        <v>0</v>
-      </c>
-      <c r="N33" s="4">
-        <v>1</v>
-      </c>
-      <c r="O33" s="4">
+      <c r="L33" s="2">
+        <v>1</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1</v>
+      </c>
+      <c r="O33" s="2">
         <v>2.9848059841047201</v>
       </c>
-      <c r="P33" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="4" t="s">
+      <c r="P33" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R33" s="4">
+      <c r="R33" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1023</v>
       </c>
@@ -3343,63 +3352,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+    <row r="35" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>1024</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="2">
         <v>12893</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="2">
         <v>74</v>
       </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="4">
-        <v>1</v>
-      </c>
-      <c r="H35" s="4">
-        <v>0</v>
-      </c>
-      <c r="I35" s="4">
-        <v>0</v>
-      </c>
-      <c r="J35" s="4">
-        <v>0</v>
-      </c>
-      <c r="K35" s="4">
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
         <v>14.3970944309927</v>
       </c>
-      <c r="L35" s="4">
-        <v>1</v>
-      </c>
-      <c r="M35" s="4">
-        <v>0</v>
-      </c>
-      <c r="N35" s="4">
-        <v>1</v>
-      </c>
-      <c r="O35" s="4">
+      <c r="L35" s="2">
+        <v>1</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0</v>
+      </c>
+      <c r="N35" s="2">
+        <v>1</v>
+      </c>
+      <c r="O35" s="2">
         <v>2.3384615384615302</v>
       </c>
-      <c r="P35" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="4" t="s">
+      <c r="P35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R35" s="4">
+      <c r="R35" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1024</v>
       </c>
@@ -3449,7 +3458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1025</v>
       </c>
@@ -3499,7 +3508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1025</v>
       </c>
@@ -3549,7 +3558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1025</v>
       </c>
@@ -3599,7 +3608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1026</v>
       </c>
@@ -3649,63 +3658,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>1026</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41">
         <v>12904</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41">
         <v>10</v>
       </c>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2">
-        <v>0</v>
-      </c>
-      <c r="G41" s="2">
-        <v>1</v>
-      </c>
-      <c r="H41" s="2">
-        <v>0</v>
-      </c>
-      <c r="I41" s="2">
-        <v>1</v>
-      </c>
-      <c r="J41" s="2">
-        <v>1</v>
-      </c>
-      <c r="K41" s="2">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
         <v>7.7512764405543297</v>
       </c>
-      <c r="L41" s="2">
-        <v>1</v>
-      </c>
-      <c r="M41" s="2">
-        <v>0</v>
-      </c>
-      <c r="N41" s="2">
-        <v>1</v>
-      </c>
-      <c r="O41" s="2">
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
         <v>2</v>
       </c>
-      <c r="P41" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="R41" s="2">
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>252</v>
+      </c>
+      <c r="R41">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1027</v>
       </c>
@@ -3755,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1027</v>
       </c>
@@ -3805,63 +3814,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>1028</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44">
         <v>12914</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44">
         <v>22</v>
       </c>
-      <c r="E44" s="2">
-        <v>0</v>
-      </c>
-      <c r="F44" s="2">
-        <v>0</v>
-      </c>
-      <c r="G44" s="2">
-        <v>1</v>
-      </c>
-      <c r="H44" s="2">
-        <v>0</v>
-      </c>
-      <c r="I44" s="2">
-        <v>1</v>
-      </c>
-      <c r="J44" s="2">
-        <v>1</v>
-      </c>
-      <c r="K44" s="2">
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
         <v>7.3807501769285198</v>
       </c>
-      <c r="L44" s="2">
-        <v>1</v>
-      </c>
-      <c r="M44" s="2">
-        <v>0</v>
-      </c>
-      <c r="N44" s="2">
-        <v>1</v>
-      </c>
-      <c r="O44" s="2">
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44">
         <v>2</v>
       </c>
-      <c r="P44" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R44" s="2">
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>251</v>
+      </c>
+      <c r="R44">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1028</v>
       </c>
@@ -3911,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1029</v>
       </c>
@@ -3961,7 +3970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1029</v>
       </c>
@@ -4011,7 +4020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1030</v>
       </c>
@@ -4061,7 +4070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1030</v>
       </c>
@@ -4111,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1030</v>
       </c>
@@ -4161,7 +4170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1030</v>
       </c>
@@ -4211,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1031</v>
       </c>
@@ -4261,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1031</v>
       </c>
@@ -4311,63 +4320,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>1032</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54">
         <v>12939</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" t="s">
         <v>68</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54">
         <v>81</v>
       </c>
-      <c r="E54" s="2">
-        <v>0</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0</v>
-      </c>
-      <c r="G54" s="2">
-        <v>1</v>
-      </c>
-      <c r="H54" s="2">
-        <v>0</v>
-      </c>
-      <c r="I54" s="2">
-        <v>1</v>
-      </c>
-      <c r="J54" s="2">
-        <v>1</v>
-      </c>
-      <c r="K54" s="2">
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="K54">
         <v>7.8258416034247897</v>
       </c>
-      <c r="L54" s="2">
-        <v>1</v>
-      </c>
-      <c r="M54" s="2">
-        <v>0</v>
-      </c>
-      <c r="N54" s="2">
-        <v>1</v>
-      </c>
-      <c r="O54" s="2">
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
         <v>2</v>
       </c>
-      <c r="P54" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R54" s="2">
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>251</v>
+      </c>
+      <c r="R54">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1032</v>
       </c>
@@ -4417,7 +4426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1033</v>
       </c>
@@ -4467,7 +4476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1033</v>
       </c>
@@ -4517,59 +4526,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+    <row r="58" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>1034</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58" s="2">
         <v>12951</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="2">
         <v>158</v>
       </c>
-      <c r="E58" s="4">
-        <v>0</v>
-      </c>
-      <c r="F58" s="4">
-        <v>1</v>
-      </c>
-      <c r="G58" s="4">
-        <v>1</v>
-      </c>
-      <c r="H58" s="4">
-        <v>0</v>
-      </c>
-      <c r="I58" s="4">
-        <v>0</v>
-      </c>
-      <c r="J58" s="4">
-        <v>0</v>
-      </c>
-      <c r="K58" s="4">
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2">
+        <v>0</v>
+      </c>
+      <c r="K58" s="2">
         <v>8.6666666666666607</v>
       </c>
-      <c r="L58" s="4">
-        <v>1</v>
-      </c>
-      <c r="M58" s="4">
-        <v>0</v>
-      </c>
-      <c r="N58" s="4">
-        <v>1</v>
-      </c>
-      <c r="O58" s="4">
+      <c r="L58" s="2">
+        <v>1</v>
+      </c>
+      <c r="M58" s="2">
+        <v>0</v>
+      </c>
+      <c r="N58" s="2">
+        <v>1</v>
+      </c>
+      <c r="O58" s="2">
         <v>2.9848059841047201</v>
       </c>
-      <c r="P58" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="4" t="s">
+      <c r="P58" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R58" s="4">
+      <c r="R58" s="2">
         <v>13</v>
       </c>
     </row>
@@ -4629,7 +4638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1034</v>
       </c>
@@ -4679,7 +4688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1034</v>
       </c>
@@ -4729,7 +4738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1034</v>
       </c>
@@ -4779,7 +4788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1034</v>
       </c>
@@ -4829,7 +4838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1035</v>
       </c>
@@ -4879,7 +4888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1035</v>
       </c>
@@ -4929,7 +4938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1036</v>
       </c>
@@ -4979,7 +4988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1036</v>
       </c>
@@ -5029,7 +5038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1037</v>
       </c>
@@ -5079,7 +5088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1037</v>
       </c>
@@ -5129,7 +5138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1038</v>
       </c>
@@ -5179,7 +5188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1038</v>
       </c>
@@ -5229,7 +5238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1039</v>
       </c>
@@ -5279,7 +5288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1039</v>
       </c>
@@ -5329,7 +5338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1040</v>
       </c>
@@ -5379,7 +5388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>1040</v>
       </c>
@@ -5435,7 +5444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1041</v>
       </c>
@@ -5485,63 +5494,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>1041</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77">
         <v>12985</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" t="s">
         <v>91</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77">
         <v>32</v>
       </c>
-      <c r="E77" s="2">
-        <v>1</v>
-      </c>
-      <c r="F77" s="2">
-        <v>0</v>
-      </c>
-      <c r="G77" s="2">
-        <v>1</v>
-      </c>
-      <c r="H77" s="2">
-        <v>0</v>
-      </c>
-      <c r="I77" s="2">
-        <v>1</v>
-      </c>
-      <c r="J77" s="2">
-        <v>1</v>
-      </c>
-      <c r="K77" s="2">
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>1</v>
+      </c>
+      <c r="K77">
         <v>16.7789425706472</v>
       </c>
-      <c r="L77" s="2">
-        <v>1</v>
-      </c>
-      <c r="M77" s="2">
-        <v>0</v>
-      </c>
-      <c r="N77" s="2">
-        <v>1</v>
-      </c>
-      <c r="O77" s="2">
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
+      <c r="O77">
         <v>2.2675675675675602</v>
       </c>
-      <c r="P77" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q77" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="R77" s="2">
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>253</v>
+      </c>
+      <c r="R77">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1042</v>
       </c>
@@ -5591,7 +5600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1042</v>
       </c>
@@ -5641,7 +5650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>1042</v>
       </c>
@@ -5697,7 +5706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1043</v>
       </c>
@@ -5747,7 +5756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1043</v>
       </c>
@@ -5797,7 +5806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1044</v>
       </c>
@@ -5847,63 +5856,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>1044</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84">
         <v>13002</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" t="s">
         <v>98</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84">
         <v>138</v>
       </c>
-      <c r="E84" s="2">
-        <v>1</v>
-      </c>
-      <c r="F84" s="2">
-        <v>0</v>
-      </c>
-      <c r="G84" s="2">
-        <v>1</v>
-      </c>
-      <c r="H84" s="2">
-        <v>0</v>
-      </c>
-      <c r="I84" s="2">
-        <v>1</v>
-      </c>
-      <c r="J84" s="2">
-        <v>1</v>
-      </c>
-      <c r="K84" s="2">
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+      <c r="K84">
         <v>9.7531152647975006</v>
       </c>
-      <c r="L84" s="2">
-        <v>1</v>
-      </c>
-      <c r="M84" s="2">
-        <v>0</v>
-      </c>
-      <c r="N84" s="2">
-        <v>1</v>
-      </c>
-      <c r="O84" s="2">
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="N84">
+        <v>1</v>
+      </c>
+      <c r="O84">
         <v>2</v>
       </c>
-      <c r="P84" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q84" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R84" s="2">
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>251</v>
+      </c>
+      <c r="R84">
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1044</v>
       </c>
@@ -5953,7 +5962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1045</v>
       </c>
@@ -6003,7 +6012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1045</v>
       </c>
@@ -6053,7 +6062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1046</v>
       </c>
@@ -6103,7 +6112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1046</v>
       </c>
@@ -6153,7 +6162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1046</v>
       </c>
@@ -6203,7 +6212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1047</v>
       </c>
@@ -6253,7 +6262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1047</v>
       </c>
@@ -6303,7 +6312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1048</v>
       </c>
@@ -6353,7 +6362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1048</v>
       </c>
@@ -6403,7 +6412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1049</v>
       </c>
@@ -6453,7 +6462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1049</v>
       </c>
@@ -6503,7 +6512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1050</v>
       </c>
@@ -6553,7 +6562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1050</v>
       </c>
@@ -6603,7 +6612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1050</v>
       </c>
@@ -6653,7 +6662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1050</v>
       </c>
@@ -6703,7 +6712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1051</v>
       </c>
@@ -6753,7 +6762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1051</v>
       </c>
@@ -6803,7 +6812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1052</v>
       </c>
@@ -6853,7 +6862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1052</v>
       </c>
@@ -6903,7 +6912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1052</v>
       </c>
@@ -6953,63 +6962,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
+    <row r="106" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
         <v>1053</v>
       </c>
-      <c r="B106" s="4">
+      <c r="B106" s="2">
         <v>13075</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D106" s="2">
         <v>66</v>
       </c>
-      <c r="E106" s="4">
-        <v>0</v>
-      </c>
-      <c r="F106" s="4">
-        <v>1</v>
-      </c>
-      <c r="G106" s="4">
-        <v>1</v>
-      </c>
-      <c r="H106" s="4">
-        <v>0</v>
-      </c>
-      <c r="I106" s="4">
-        <v>0</v>
-      </c>
-      <c r="J106" s="4">
-        <v>0</v>
-      </c>
-      <c r="K106" s="4">
+      <c r="E106" s="2">
+        <v>0</v>
+      </c>
+      <c r="F106" s="2">
+        <v>1</v>
+      </c>
+      <c r="G106" s="2">
+        <v>1</v>
+      </c>
+      <c r="H106" s="2">
+        <v>0</v>
+      </c>
+      <c r="I106" s="2">
+        <v>0</v>
+      </c>
+      <c r="J106" s="2">
+        <v>0</v>
+      </c>
+      <c r="K106" s="2">
         <v>7.6369426751592302</v>
       </c>
-      <c r="L106" s="4">
-        <v>1</v>
-      </c>
-      <c r="M106" s="4">
-        <v>0</v>
-      </c>
-      <c r="N106" s="4">
-        <v>1</v>
-      </c>
-      <c r="O106" s="4">
+      <c r="L106" s="2">
+        <v>1</v>
+      </c>
+      <c r="M106" s="2">
+        <v>0</v>
+      </c>
+      <c r="N106" s="2">
+        <v>1</v>
+      </c>
+      <c r="O106" s="2">
         <v>2.8132701421800901</v>
       </c>
-      <c r="P106" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q106" s="4" t="s">
+      <c r="P106" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q106" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R106" s="4">
+      <c r="R106" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1053</v>
       </c>
@@ -7059,63 +7068,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+    <row r="108" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
         <v>1053</v>
       </c>
-      <c r="B108" s="4">
+      <c r="B108" s="2">
         <v>13077</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D108" s="2">
         <v>69</v>
       </c>
-      <c r="E108" s="4">
-        <v>0</v>
-      </c>
-      <c r="F108" s="4">
+      <c r="E108" s="2">
+        <v>0</v>
+      </c>
+      <c r="F108" s="2">
         <v>2</v>
       </c>
-      <c r="G108" s="4">
-        <v>0</v>
-      </c>
-      <c r="H108" s="4">
-        <v>1</v>
-      </c>
-      <c r="I108" s="4">
-        <v>0</v>
-      </c>
-      <c r="J108" s="4">
-        <v>0</v>
-      </c>
-      <c r="K108" s="4">
+      <c r="G108" s="2">
+        <v>0</v>
+      </c>
+      <c r="H108" s="2">
+        <v>1</v>
+      </c>
+      <c r="I108" s="2">
+        <v>0</v>
+      </c>
+      <c r="J108" s="2">
+        <v>0</v>
+      </c>
+      <c r="K108" s="2">
         <v>2</v>
       </c>
-      <c r="L108" s="4">
-        <v>1</v>
-      </c>
-      <c r="M108" s="4">
-        <v>0</v>
-      </c>
-      <c r="N108" s="4">
-        <v>0</v>
-      </c>
-      <c r="O108" s="4">
+      <c r="L108" s="2">
+        <v>1</v>
+      </c>
+      <c r="M108" s="2">
+        <v>0</v>
+      </c>
+      <c r="N108" s="2">
+        <v>0</v>
+      </c>
+      <c r="O108" s="2">
         <v>2.3098591549295699</v>
       </c>
-      <c r="P108" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q108" s="4" t="s">
+      <c r="P108" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q108" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R108" s="4">
+      <c r="R108" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1054</v>
       </c>
@@ -7165,7 +7174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1054</v>
       </c>
@@ -7215,7 +7224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1054</v>
       </c>
@@ -7265,63 +7274,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112">
         <v>1055</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112">
         <v>13089</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" t="s">
         <v>125</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112">
         <v>27</v>
       </c>
-      <c r="E112" s="2">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2">
-        <v>0</v>
-      </c>
-      <c r="G112" s="2">
-        <v>1</v>
-      </c>
-      <c r="H112" s="2">
-        <v>0</v>
-      </c>
-      <c r="I112" s="2">
-        <v>1</v>
-      </c>
-      <c r="J112" s="2">
-        <v>1</v>
-      </c>
-      <c r="K112" s="2">
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+      <c r="K112">
         <v>9.4319848592382307</v>
       </c>
-      <c r="L112" s="2">
-        <v>1</v>
-      </c>
-      <c r="M112" s="2">
-        <v>0</v>
-      </c>
-      <c r="N112" s="2">
-        <v>1</v>
-      </c>
-      <c r="O112" s="2">
+      <c r="L112">
+        <v>1</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+      <c r="N112">
+        <v>1</v>
+      </c>
+      <c r="O112">
         <v>2</v>
       </c>
-      <c r="P112" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q112" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R112" s="2">
+      <c r="P112">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>251</v>
+      </c>
+      <c r="R112">
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1055</v>
       </c>
@@ -7371,63 +7380,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114">
         <v>1055</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114">
         <v>13091</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" t="s">
         <v>127</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D114">
         <v>12</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114">
         <v>2</v>
       </c>
-      <c r="F114" s="2">
-        <v>0</v>
-      </c>
-      <c r="G114" s="2">
-        <v>1</v>
-      </c>
-      <c r="H114" s="2">
-        <v>0</v>
-      </c>
-      <c r="I114" s="2">
-        <v>1</v>
-      </c>
-      <c r="J114" s="2">
-        <v>1</v>
-      </c>
-      <c r="K114" s="2">
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>1</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>1</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="K114">
         <v>43.4625850340136</v>
       </c>
-      <c r="L114" s="2">
-        <v>1</v>
-      </c>
-      <c r="M114" s="2">
-        <v>0</v>
-      </c>
-      <c r="N114" s="2">
-        <v>1</v>
-      </c>
-      <c r="O114" s="2">
+      <c r="L114">
+        <v>1</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="N114">
+        <v>1</v>
+      </c>
+      <c r="O114">
         <v>2</v>
       </c>
-      <c r="P114" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q114" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R114" s="2">
+      <c r="P114">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>251</v>
+      </c>
+      <c r="R114">
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1056</v>
       </c>
@@ -7477,7 +7486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1056</v>
       </c>
@@ -7527,7 +7536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1057</v>
       </c>
@@ -7577,7 +7586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1057</v>
       </c>
@@ -7627,7 +7636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1058</v>
       </c>
@@ -7677,7 +7686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1058</v>
       </c>
@@ -7727,7 +7736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1058</v>
       </c>
@@ -7777,7 +7786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>1058</v>
       </c>
@@ -7833,7 +7842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>1058</v>
       </c>
@@ -7883,7 +7892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>1058</v>
       </c>
@@ -7933,7 +7942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1058</v>
       </c>
@@ -7983,7 +7992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>1058</v>
       </c>
@@ -8033,7 +8042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>1058</v>
       </c>
@@ -8083,7 +8092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1059</v>
       </c>
@@ -8133,7 +8142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1059</v>
       </c>
@@ -8183,63 +8192,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
+    <row r="130" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
         <v>1060</v>
       </c>
-      <c r="B130" s="4">
+      <c r="B130" s="2">
         <v>13161</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C130" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D130" s="2">
         <v>119</v>
       </c>
-      <c r="E130" s="4">
-        <v>0</v>
-      </c>
-      <c r="F130" s="4">
-        <v>0</v>
-      </c>
-      <c r="G130" s="4">
-        <v>1</v>
-      </c>
-      <c r="H130" s="4">
-        <v>0</v>
-      </c>
-      <c r="I130" s="4">
-        <v>1</v>
-      </c>
-      <c r="J130" s="4">
-        <v>1</v>
-      </c>
-      <c r="K130" s="4">
+      <c r="E130" s="2">
+        <v>0</v>
+      </c>
+      <c r="F130" s="2">
+        <v>0</v>
+      </c>
+      <c r="G130" s="2">
+        <v>1</v>
+      </c>
+      <c r="H130" s="2">
+        <v>0</v>
+      </c>
+      <c r="I130" s="2">
+        <v>1</v>
+      </c>
+      <c r="J130" s="2">
+        <v>1</v>
+      </c>
+      <c r="K130" s="2">
         <v>7.29295652592557</v>
       </c>
-      <c r="L130" s="4">
-        <v>1</v>
-      </c>
-      <c r="M130" s="4">
-        <v>0</v>
-      </c>
-      <c r="N130" s="4">
-        <v>1</v>
-      </c>
-      <c r="O130" s="4">
+      <c r="L130" s="2">
+        <v>1</v>
+      </c>
+      <c r="M130" s="2">
+        <v>0</v>
+      </c>
+      <c r="N130" s="2">
+        <v>1</v>
+      </c>
+      <c r="O130" s="2">
         <v>2.0897552130552999</v>
       </c>
-      <c r="P130" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q130" s="4" t="s">
+      <c r="P130" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R130" s="4">
+      <c r="R130" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>1060</v>
       </c>
@@ -8289,7 +8298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1061</v>
       </c>
@@ -8339,63 +8348,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133">
         <v>1061</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B133">
         <v>13172</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" t="s">
         <v>146</v>
       </c>
-      <c r="D133" s="2">
+      <c r="D133">
         <v>32</v>
       </c>
-      <c r="E133" s="2">
-        <v>0</v>
-      </c>
-      <c r="F133" s="2">
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
         <v>2</v>
       </c>
-      <c r="G133" s="2">
-        <v>0</v>
-      </c>
-      <c r="H133" s="2">
-        <v>0</v>
-      </c>
-      <c r="I133" s="2">
-        <v>1</v>
-      </c>
-      <c r="J133" s="2">
-        <v>0</v>
-      </c>
-      <c r="K133" s="2">
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+      <c r="K133">
         <v>2.8877928483353799</v>
       </c>
-      <c r="L133" s="2">
-        <v>0</v>
-      </c>
-      <c r="M133" s="2">
-        <v>0</v>
-      </c>
-      <c r="N133" s="2">
-        <v>1</v>
-      </c>
-      <c r="O133" s="2">
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133">
+        <v>0</v>
+      </c>
+      <c r="N133">
+        <v>1</v>
+      </c>
+      <c r="O133">
         <v>2</v>
       </c>
-      <c r="P133" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q133" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="R133" s="2">
+      <c r="P133">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>252</v>
+      </c>
+      <c r="R133">
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>1061</v>
       </c>
@@ -8445,7 +8454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1061</v>
       </c>
@@ -8495,7 +8504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1062</v>
       </c>
@@ -8545,7 +8554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1062</v>
       </c>
@@ -8595,7 +8604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1063</v>
       </c>
@@ -8645,7 +8654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>1063</v>
       </c>
@@ -8701,7 +8710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1064</v>
       </c>
@@ -8751,7 +8760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>1064</v>
       </c>
@@ -8801,7 +8810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>1065</v>
       </c>
@@ -8851,7 +8860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1065</v>
       </c>
@@ -8901,7 +8910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>1066</v>
       </c>
@@ -8951,7 +8960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>1066</v>
       </c>
@@ -9001,7 +9010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1067</v>
       </c>
@@ -9051,7 +9060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>1067</v>
       </c>
@@ -9101,7 +9110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>1067</v>
       </c>
@@ -9157,7 +9166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>1067</v>
       </c>
@@ -9207,7 +9216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1068</v>
       </c>
@@ -9257,7 +9266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1068</v>
       </c>
@@ -9307,7 +9316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1068</v>
       </c>
@@ -9357,63 +9366,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="2">
+    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A153">
         <v>1069</v>
       </c>
-      <c r="B153" s="2">
+      <c r="B153">
         <v>13218</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C153" t="s">
         <v>166</v>
       </c>
-      <c r="D153" s="2">
+      <c r="D153">
         <v>18</v>
       </c>
-      <c r="E153" s="2">
-        <v>0</v>
-      </c>
-      <c r="F153" s="2">
-        <v>0</v>
-      </c>
-      <c r="G153" s="2">
-        <v>1</v>
-      </c>
-      <c r="H153" s="2">
-        <v>0</v>
-      </c>
-      <c r="I153" s="2">
-        <v>1</v>
-      </c>
-      <c r="J153" s="2">
-        <v>1</v>
-      </c>
-      <c r="K153" s="2">
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
+      </c>
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>1</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="K153">
         <v>7</v>
       </c>
-      <c r="L153" s="2">
-        <v>1</v>
-      </c>
-      <c r="M153" s="2">
-        <v>0</v>
-      </c>
-      <c r="N153" s="2">
-        <v>1</v>
-      </c>
-      <c r="O153" s="2">
+      <c r="L153">
+        <v>1</v>
+      </c>
+      <c r="M153">
+        <v>0</v>
+      </c>
+      <c r="N153">
+        <v>1</v>
+      </c>
+      <c r="O153">
         <v>2</v>
       </c>
-      <c r="P153" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q153" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="R153" s="2">
+      <c r="P153">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>252</v>
+      </c>
+      <c r="R153">
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1069</v>
       </c>
@@ -9463,7 +9472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1070</v>
       </c>
@@ -9513,7 +9522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1070</v>
       </c>
@@ -9563,7 +9572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1071</v>
       </c>
@@ -9613,7 +9622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1071</v>
       </c>
@@ -9663,7 +9672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1072</v>
       </c>
@@ -9713,7 +9722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1072</v>
       </c>
@@ -9763,7 +9772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1073</v>
       </c>
@@ -9813,7 +9822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1073</v>
       </c>
@@ -9863,175 +9872,175 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="4">
+    <row r="163" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
         <v>1074</v>
       </c>
-      <c r="B163" s="4">
+      <c r="B163" s="2">
         <v>13239</v>
       </c>
-      <c r="C163" s="4" t="s">
+      <c r="C163" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D163" s="2">
         <v>95</v>
       </c>
-      <c r="E163" s="4">
-        <v>0</v>
-      </c>
-      <c r="F163" s="4">
-        <v>0</v>
-      </c>
-      <c r="G163" s="4">
-        <v>1</v>
-      </c>
-      <c r="H163" s="4">
-        <v>0</v>
-      </c>
-      <c r="I163" s="4">
-        <v>1</v>
-      </c>
-      <c r="J163" s="4">
-        <v>1</v>
-      </c>
-      <c r="K163" s="4">
+      <c r="E163" s="2">
+        <v>0</v>
+      </c>
+      <c r="F163" s="2">
+        <v>0</v>
+      </c>
+      <c r="G163" s="2">
+        <v>1</v>
+      </c>
+      <c r="H163" s="2">
+        <v>0</v>
+      </c>
+      <c r="I163" s="2">
+        <v>1</v>
+      </c>
+      <c r="J163" s="2">
+        <v>1</v>
+      </c>
+      <c r="K163" s="2">
         <v>9.8671291355389492</v>
       </c>
-      <c r="L163" s="4">
-        <v>1</v>
-      </c>
-      <c r="M163" s="4">
-        <v>0</v>
-      </c>
-      <c r="N163" s="4">
-        <v>1</v>
-      </c>
-      <c r="O163" s="4">
+      <c r="L163" s="2">
+        <v>1</v>
+      </c>
+      <c r="M163" s="2">
+        <v>0</v>
+      </c>
+      <c r="N163" s="2">
+        <v>1</v>
+      </c>
+      <c r="O163" s="2">
         <v>2</v>
       </c>
-      <c r="P163" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q163" s="4" t="s">
+      <c r="P163" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q163" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R163" s="4">
+      <c r="R163" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="4">
+    <row r="164" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
         <v>1074</v>
       </c>
-      <c r="B164" s="4">
+      <c r="B164" s="2">
         <v>13240</v>
       </c>
-      <c r="C164" s="4" t="s">
+      <c r="C164" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D164" s="2">
         <v>61</v>
       </c>
-      <c r="E164" s="4">
-        <v>1</v>
-      </c>
-      <c r="F164" s="4">
-        <v>0</v>
-      </c>
-      <c r="G164" s="4">
-        <v>1</v>
-      </c>
-      <c r="H164" s="4">
-        <v>0</v>
-      </c>
-      <c r="I164" s="4">
-        <v>1</v>
-      </c>
-      <c r="J164" s="4">
-        <v>1</v>
-      </c>
-      <c r="K164" s="4">
+      <c r="E164" s="2">
+        <v>1</v>
+      </c>
+      <c r="F164" s="2">
+        <v>0</v>
+      </c>
+      <c r="G164" s="2">
+        <v>1</v>
+      </c>
+      <c r="H164" s="2">
+        <v>0</v>
+      </c>
+      <c r="I164" s="2">
+        <v>1</v>
+      </c>
+      <c r="J164" s="2">
+        <v>1</v>
+      </c>
+      <c r="K164" s="2">
         <v>4.8671291355389501</v>
       </c>
-      <c r="L164" s="4">
-        <v>1</v>
-      </c>
-      <c r="M164" s="4">
-        <v>0</v>
-      </c>
-      <c r="N164" s="4">
-        <v>1</v>
-      </c>
-      <c r="O164" s="4">
+      <c r="L164" s="2">
+        <v>1</v>
+      </c>
+      <c r="M164" s="2">
+        <v>0</v>
+      </c>
+      <c r="N164" s="2">
+        <v>1</v>
+      </c>
+      <c r="O164" s="2">
         <v>2</v>
       </c>
-      <c r="P164" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q164" s="4" t="s">
+      <c r="P164" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q164" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R164" s="4">
+      <c r="R164" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="4">
+    <row r="165" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
         <v>1074</v>
       </c>
-      <c r="B165" s="4">
+      <c r="B165" s="2">
         <v>13241</v>
       </c>
-      <c r="C165" s="4" t="s">
+      <c r="C165" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D165" s="2">
         <v>106</v>
       </c>
-      <c r="E165" s="4">
+      <c r="E165" s="2">
         <v>2</v>
       </c>
-      <c r="F165" s="4">
-        <v>0</v>
-      </c>
-      <c r="G165" s="4">
-        <v>1</v>
-      </c>
-      <c r="H165" s="4">
-        <v>0</v>
-      </c>
-      <c r="I165" s="4">
-        <v>1</v>
-      </c>
-      <c r="J165" s="4">
-        <v>1</v>
-      </c>
-      <c r="K165" s="4">
+      <c r="F165" s="2">
+        <v>0</v>
+      </c>
+      <c r="G165" s="2">
+        <v>1</v>
+      </c>
+      <c r="H165" s="2">
+        <v>0</v>
+      </c>
+      <c r="I165" s="2">
+        <v>1</v>
+      </c>
+      <c r="J165" s="2">
+        <v>1</v>
+      </c>
+      <c r="K165" s="2">
         <v>10.3777777777777</v>
       </c>
-      <c r="L165" s="4">
-        <v>1</v>
-      </c>
-      <c r="M165" s="4">
-        <v>0</v>
-      </c>
-      <c r="N165" s="4">
-        <v>1</v>
-      </c>
-      <c r="O165" s="4">
+      <c r="L165" s="2">
+        <v>1</v>
+      </c>
+      <c r="M165" s="2">
+        <v>0</v>
+      </c>
+      <c r="N165" s="2">
+        <v>1</v>
+      </c>
+      <c r="O165" s="2">
         <v>2</v>
       </c>
-      <c r="P165" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q165" s="4" t="s">
+      <c r="P165" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q165" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R165" s="4">
+      <c r="R165" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1074</v>
       </c>
@@ -10081,7 +10090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1075</v>
       </c>
@@ -10131,63 +10140,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="4">
+    <row r="168" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
         <v>1075</v>
       </c>
-      <c r="B168" s="4">
+      <c r="B168" s="2">
         <v>13245</v>
       </c>
-      <c r="C168" s="4" t="s">
+      <c r="C168" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D168" s="2">
         <v>98</v>
       </c>
-      <c r="E168" s="4">
-        <v>1</v>
-      </c>
-      <c r="F168" s="4">
-        <v>0</v>
-      </c>
-      <c r="G168" s="4">
-        <v>1</v>
-      </c>
-      <c r="H168" s="4">
-        <v>0</v>
-      </c>
-      <c r="I168" s="4">
-        <v>1</v>
-      </c>
-      <c r="J168" s="4">
-        <v>1</v>
-      </c>
-      <c r="K168" s="4">
+      <c r="E168" s="2">
+        <v>1</v>
+      </c>
+      <c r="F168" s="2">
+        <v>0</v>
+      </c>
+      <c r="G168" s="2">
+        <v>1</v>
+      </c>
+      <c r="H168" s="2">
+        <v>0</v>
+      </c>
+      <c r="I168" s="2">
+        <v>1</v>
+      </c>
+      <c r="J168" s="2">
+        <v>1</v>
+      </c>
+      <c r="K168" s="2">
         <v>82</v>
       </c>
-      <c r="L168" s="4">
-        <v>1</v>
-      </c>
-      <c r="M168" s="4">
-        <v>0</v>
-      </c>
-      <c r="N168" s="4">
-        <v>1</v>
-      </c>
-      <c r="O168" s="4">
-        <v>0</v>
-      </c>
-      <c r="P168" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q168" s="4" t="s">
+      <c r="L168" s="2">
+        <v>1</v>
+      </c>
+      <c r="M168" s="2">
+        <v>0</v>
+      </c>
+      <c r="N168" s="2">
+        <v>1</v>
+      </c>
+      <c r="O168" s="2">
+        <v>0</v>
+      </c>
+      <c r="P168" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q168" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R168" s="4">
+      <c r="R168" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1075</v>
       </c>
@@ -10237,7 +10246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>1076</v>
       </c>
@@ -10287,7 +10296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>1076</v>
       </c>
@@ -10337,7 +10346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1077</v>
       </c>
@@ -10387,63 +10396,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="4">
+    <row r="173" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
         <v>1077</v>
       </c>
-      <c r="B173" s="4">
+      <c r="B173" s="2">
         <v>13262</v>
       </c>
-      <c r="C173" s="4" t="s">
+      <c r="C173" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D173" s="2">
         <v>46</v>
       </c>
-      <c r="E173" s="4">
-        <v>0</v>
-      </c>
-      <c r="F173" s="4">
-        <v>1</v>
-      </c>
-      <c r="G173" s="4">
-        <v>1</v>
-      </c>
-      <c r="H173" s="4">
-        <v>0</v>
-      </c>
-      <c r="I173" s="4">
-        <v>0</v>
-      </c>
-      <c r="J173" s="4">
-        <v>0</v>
-      </c>
-      <c r="K173" s="4">
+      <c r="E173" s="2">
+        <v>0</v>
+      </c>
+      <c r="F173" s="2">
+        <v>1</v>
+      </c>
+      <c r="G173" s="2">
+        <v>1</v>
+      </c>
+      <c r="H173" s="2">
+        <v>0</v>
+      </c>
+      <c r="I173" s="2">
+        <v>0</v>
+      </c>
+      <c r="J173" s="2">
+        <v>0</v>
+      </c>
+      <c r="K173" s="2">
         <v>1.6438356164383501</v>
       </c>
-      <c r="L173" s="4">
-        <v>0</v>
-      </c>
-      <c r="M173" s="4">
-        <v>0</v>
-      </c>
-      <c r="N173" s="4">
-        <v>1</v>
-      </c>
-      <c r="O173" s="4">
+      <c r="L173" s="2">
+        <v>0</v>
+      </c>
+      <c r="M173" s="2">
+        <v>0</v>
+      </c>
+      <c r="N173" s="2">
+        <v>1</v>
+      </c>
+      <c r="O173" s="2">
         <v>2</v>
       </c>
-      <c r="P173" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q173" s="4" t="s">
+      <c r="P173" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q173" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R173" s="4">
+      <c r="R173" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1077</v>
       </c>
@@ -10493,7 +10502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1078</v>
       </c>
@@ -10543,7 +10552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1078</v>
       </c>
@@ -10593,7 +10602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1079</v>
       </c>
@@ -10643,7 +10652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1079</v>
       </c>
@@ -10693,63 +10702,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="4">
+    <row r="179" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
         <v>1080</v>
       </c>
-      <c r="B179" s="4">
+      <c r="B179" s="2">
         <v>13308</v>
       </c>
-      <c r="C179" s="4" t="s">
+      <c r="C179" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D179" s="2">
         <v>11</v>
       </c>
-      <c r="E179" s="4">
-        <v>0</v>
-      </c>
-      <c r="F179" s="4">
-        <v>0</v>
-      </c>
-      <c r="G179" s="4">
-        <v>1</v>
-      </c>
-      <c r="H179" s="4">
-        <v>0</v>
-      </c>
-      <c r="I179" s="4">
-        <v>1</v>
-      </c>
-      <c r="J179" s="4">
-        <v>1</v>
-      </c>
-      <c r="K179" s="4">
+      <c r="E179" s="2">
+        <v>0</v>
+      </c>
+      <c r="F179" s="2">
+        <v>0</v>
+      </c>
+      <c r="G179" s="2">
+        <v>1</v>
+      </c>
+      <c r="H179" s="2">
+        <v>0</v>
+      </c>
+      <c r="I179" s="2">
+        <v>1</v>
+      </c>
+      <c r="J179" s="2">
+        <v>1</v>
+      </c>
+      <c r="K179" s="2">
         <v>13.3095238095238</v>
       </c>
-      <c r="L179" s="4">
-        <v>1</v>
-      </c>
-      <c r="M179" s="4">
-        <v>0</v>
-      </c>
-      <c r="N179" s="4">
-        <v>1</v>
-      </c>
-      <c r="O179" s="4">
+      <c r="L179" s="2">
+        <v>1</v>
+      </c>
+      <c r="M179" s="2">
+        <v>0</v>
+      </c>
+      <c r="N179" s="2">
+        <v>1</v>
+      </c>
+      <c r="O179" s="2">
         <v>2.1769606434932398</v>
       </c>
-      <c r="P179" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q179" s="4" t="s">
+      <c r="P179" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q179" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R179" s="4">
+      <c r="R179" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1080</v>
       </c>
@@ -10799,7 +10808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>1081</v>
       </c>
@@ -10849,7 +10858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>1081</v>
       </c>
@@ -10899,63 +10908,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="2">
+    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A183">
         <v>1082</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B183">
         <v>13326</v>
       </c>
-      <c r="C183" s="2">
+      <c r="C183">
         <v>17071</v>
       </c>
-      <c r="D183" s="2">
+      <c r="D183">
         <v>5</v>
       </c>
-      <c r="E183" s="2">
-        <v>0</v>
-      </c>
-      <c r="F183" s="2">
-        <v>0</v>
-      </c>
-      <c r="G183" s="2">
-        <v>1</v>
-      </c>
-      <c r="H183" s="2">
-        <v>0</v>
-      </c>
-      <c r="I183" s="2">
-        <v>1</v>
-      </c>
-      <c r="J183" s="2">
-        <v>1</v>
-      </c>
-      <c r="K183" s="2">
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183">
+        <v>1</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183">
+        <v>1</v>
+      </c>
+      <c r="J183">
+        <v>1</v>
+      </c>
+      <c r="K183">
         <v>7</v>
       </c>
-      <c r="L183" s="2">
-        <v>1</v>
-      </c>
-      <c r="M183" s="2">
-        <v>0</v>
-      </c>
-      <c r="N183" s="2">
-        <v>1</v>
-      </c>
-      <c r="O183" s="2">
+      <c r="L183">
+        <v>1</v>
+      </c>
+      <c r="M183">
+        <v>0</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
+      <c r="O183">
         <v>2</v>
       </c>
-      <c r="P183" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q183" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="R183" s="2">
+      <c r="P183">
+        <v>0</v>
+      </c>
+      <c r="Q183" t="s">
+        <v>252</v>
+      </c>
+      <c r="R183">
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>1082</v>
       </c>
@@ -11005,7 +11014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>1083</v>
       </c>
@@ -11061,7 +11070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>1083</v>
       </c>
@@ -11111,7 +11120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>1084</v>
       </c>
@@ -11161,63 +11170,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
+    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A188">
         <v>1084</v>
       </c>
-      <c r="B188" s="2">
+      <c r="B188">
         <v>13368</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="C188" t="s">
         <v>200</v>
       </c>
-      <c r="D188" s="2">
+      <c r="D188">
         <v>176</v>
       </c>
-      <c r="E188" s="2">
-        <v>1</v>
-      </c>
-      <c r="F188" s="2">
-        <v>0</v>
-      </c>
-      <c r="G188" s="2">
-        <v>1</v>
-      </c>
-      <c r="H188" s="2">
-        <v>0</v>
-      </c>
-      <c r="I188" s="2">
-        <v>1</v>
-      </c>
-      <c r="J188" s="2">
-        <v>1</v>
-      </c>
-      <c r="K188" s="2">
+      <c r="E188">
+        <v>1</v>
+      </c>
+      <c r="F188">
+        <v>0</v>
+      </c>
+      <c r="G188">
+        <v>1</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188">
+        <v>1</v>
+      </c>
+      <c r="J188">
+        <v>1</v>
+      </c>
+      <c r="K188">
         <v>7.29295652592557</v>
       </c>
-      <c r="L188" s="2">
-        <v>1</v>
-      </c>
-      <c r="M188" s="2">
-        <v>0</v>
-      </c>
-      <c r="N188" s="2">
-        <v>1</v>
-      </c>
-      <c r="O188" s="2">
+      <c r="L188">
+        <v>1</v>
+      </c>
+      <c r="M188">
+        <v>0</v>
+      </c>
+      <c r="N188">
+        <v>1</v>
+      </c>
+      <c r="O188">
         <v>2.0723684210526301</v>
       </c>
-      <c r="P188" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q188" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R188" s="2">
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="Q188" t="s">
+        <v>251</v>
+      </c>
+      <c r="R188">
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>1085</v>
       </c>
@@ -11267,7 +11276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>1085</v>
       </c>
@@ -11317,7 +11326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1085</v>
       </c>
@@ -11367,7 +11376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>1086</v>
       </c>
@@ -11417,7 +11426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1086</v>
       </c>
@@ -11467,63 +11476,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="4">
+    <row r="194" spans="1:18" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
         <v>1086</v>
       </c>
-      <c r="B194" s="4">
+      <c r="B194" s="2">
         <v>13388</v>
       </c>
-      <c r="C194" s="4" t="s">
+      <c r="C194" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D194" s="4">
+      <c r="D194" s="2">
         <v>27</v>
       </c>
-      <c r="E194" s="4">
+      <c r="E194" s="2">
         <v>2</v>
       </c>
-      <c r="F194" s="4">
-        <v>0</v>
-      </c>
-      <c r="G194" s="4">
-        <v>1</v>
-      </c>
-      <c r="H194" s="4">
-        <v>0</v>
-      </c>
-      <c r="I194" s="4">
-        <v>1</v>
-      </c>
-      <c r="J194" s="4">
-        <v>1</v>
-      </c>
-      <c r="K194" s="4">
+      <c r="F194" s="2">
+        <v>0</v>
+      </c>
+      <c r="G194" s="2">
+        <v>1</v>
+      </c>
+      <c r="H194" s="2">
+        <v>0</v>
+      </c>
+      <c r="I194" s="2">
+        <v>1</v>
+      </c>
+      <c r="J194" s="2">
+        <v>1</v>
+      </c>
+      <c r="K194" s="2">
         <v>7.29295652592557</v>
       </c>
-      <c r="L194" s="4">
-        <v>1</v>
-      </c>
-      <c r="M194" s="4">
-        <v>0</v>
-      </c>
-      <c r="N194" s="4">
-        <v>1</v>
-      </c>
-      <c r="O194" s="4">
+      <c r="L194" s="2">
+        <v>1</v>
+      </c>
+      <c r="M194" s="2">
+        <v>0</v>
+      </c>
+      <c r="N194" s="2">
+        <v>1</v>
+      </c>
+      <c r="O194" s="2">
         <v>2</v>
       </c>
-      <c r="P194" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q194" s="4" t="s">
+      <c r="P194" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q194" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="R194" s="4">
+      <c r="R194" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>1087</v>
       </c>
@@ -11573,7 +11582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1087</v>
       </c>
@@ -11623,63 +11632,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A197">
         <v>1088</v>
       </c>
-      <c r="B197" s="2">
+      <c r="B197">
         <v>13405</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="C197" t="s">
         <v>209</v>
       </c>
-      <c r="D197" s="2">
+      <c r="D197">
         <v>15</v>
       </c>
-      <c r="E197" s="2">
-        <v>0</v>
-      </c>
-      <c r="F197" s="2">
-        <v>0</v>
-      </c>
-      <c r="G197" s="2">
-        <v>1</v>
-      </c>
-      <c r="H197" s="2">
-        <v>0</v>
-      </c>
-      <c r="I197" s="2">
-        <v>1</v>
-      </c>
-      <c r="J197" s="2">
-        <v>1</v>
-      </c>
-      <c r="K197" s="2">
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="G197">
+        <v>1</v>
+      </c>
+      <c r="H197">
+        <v>0</v>
+      </c>
+      <c r="I197">
+        <v>1</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+      <c r="K197">
         <v>7.2258622443788703</v>
       </c>
-      <c r="L197" s="2">
-        <v>1</v>
-      </c>
-      <c r="M197" s="2">
-        <v>0</v>
-      </c>
-      <c r="N197" s="2">
-        <v>1</v>
-      </c>
-      <c r="O197" s="2">
+      <c r="L197">
+        <v>1</v>
+      </c>
+      <c r="M197">
+        <v>0</v>
+      </c>
+      <c r="N197">
+        <v>1</v>
+      </c>
+      <c r="O197">
         <v>2</v>
       </c>
-      <c r="P197" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q197" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R197" s="2">
+      <c r="P197">
+        <v>0</v>
+      </c>
+      <c r="Q197" t="s">
+        <v>251</v>
+      </c>
+      <c r="R197">
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>1088</v>
       </c>
@@ -11729,7 +11738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>1088</v>
       </c>
@@ -11779,7 +11788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>1089</v>
       </c>
@@ -11829,7 +11838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>1089</v>
       </c>
@@ -11879,7 +11888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>1090</v>
       </c>
@@ -11929,7 +11938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>1090</v>
       </c>
@@ -11979,63 +11988,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="2">
+    <row r="204" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A204">
         <v>1091</v>
       </c>
-      <c r="B204" s="2">
+      <c r="B204">
         <v>13420</v>
       </c>
-      <c r="C204" s="2" t="s">
+      <c r="C204" t="s">
         <v>216</v>
       </c>
-      <c r="D204" s="2">
+      <c r="D204">
         <v>21</v>
       </c>
-      <c r="E204" s="2">
-        <v>0</v>
-      </c>
-      <c r="F204" s="2">
-        <v>0</v>
-      </c>
-      <c r="G204" s="2">
-        <v>1</v>
-      </c>
-      <c r="H204" s="2">
-        <v>0</v>
-      </c>
-      <c r="I204" s="2">
-        <v>1</v>
-      </c>
-      <c r="J204" s="2">
-        <v>1</v>
-      </c>
-      <c r="K204" s="2">
+      <c r="E204">
+        <v>0</v>
+      </c>
+      <c r="F204">
+        <v>0</v>
+      </c>
+      <c r="G204">
+        <v>1</v>
+      </c>
+      <c r="H204">
+        <v>0</v>
+      </c>
+      <c r="I204">
+        <v>1</v>
+      </c>
+      <c r="J204">
+        <v>1</v>
+      </c>
+      <c r="K204">
         <v>7.7512764405543297</v>
       </c>
-      <c r="L204" s="2">
-        <v>1</v>
-      </c>
-      <c r="M204" s="2">
-        <v>0</v>
-      </c>
-      <c r="N204" s="2">
-        <v>1</v>
-      </c>
-      <c r="O204" s="2">
+      <c r="L204">
+        <v>1</v>
+      </c>
+      <c r="M204">
+        <v>0</v>
+      </c>
+      <c r="N204">
+        <v>1</v>
+      </c>
+      <c r="O204">
         <v>2</v>
       </c>
-      <c r="P204" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q204" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="R204" s="2">
+      <c r="P204">
+        <v>0</v>
+      </c>
+      <c r="Q204" t="s">
+        <v>252</v>
+      </c>
+      <c r="R204">
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>1091</v>
       </c>
@@ -12085,7 +12094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>1092</v>
       </c>
@@ -12135,7 +12144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>1092</v>
       </c>
@@ -12185,7 +12194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>1093</v>
       </c>
@@ -12235,7 +12244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>1093</v>
       </c>
@@ -12285,7 +12294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>1094</v>
       </c>
@@ -12335,7 +12344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>1094</v>
       </c>
@@ -12385,7 +12394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>1095</v>
       </c>
@@ -12435,63 +12444,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="2">
+    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A213">
         <v>1095</v>
       </c>
-      <c r="B213" s="2">
+      <c r="B213">
         <v>13437</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="C213" t="s">
         <v>225</v>
       </c>
-      <c r="D213" s="2">
+      <c r="D213">
         <v>9</v>
       </c>
-      <c r="E213" s="2">
-        <v>1</v>
-      </c>
-      <c r="F213" s="2">
-        <v>0</v>
-      </c>
-      <c r="G213" s="2">
-        <v>1</v>
-      </c>
-      <c r="H213" s="2">
-        <v>0</v>
-      </c>
-      <c r="I213" s="2">
-        <v>1</v>
-      </c>
-      <c r="J213" s="2">
-        <v>1</v>
-      </c>
-      <c r="K213" s="2">
+      <c r="E213">
+        <v>1</v>
+      </c>
+      <c r="F213">
+        <v>0</v>
+      </c>
+      <c r="G213">
+        <v>1</v>
+      </c>
+      <c r="H213">
+        <v>0</v>
+      </c>
+      <c r="I213">
+        <v>1</v>
+      </c>
+      <c r="J213">
+        <v>1</v>
+      </c>
+      <c r="K213">
         <v>39.307692307692299</v>
       </c>
-      <c r="L213" s="2">
-        <v>1</v>
-      </c>
-      <c r="M213" s="2">
-        <v>0</v>
-      </c>
-      <c r="N213" s="2">
-        <v>1</v>
-      </c>
-      <c r="O213" s="2">
+      <c r="L213">
+        <v>1</v>
+      </c>
+      <c r="M213">
+        <v>0</v>
+      </c>
+      <c r="N213">
+        <v>1</v>
+      </c>
+      <c r="O213">
         <v>2</v>
       </c>
-      <c r="P213" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q213" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="R213" s="2">
+      <c r="P213">
+        <v>0</v>
+      </c>
+      <c r="Q213" t="s">
+        <v>251</v>
+      </c>
+      <c r="R213">
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>1096</v>
       </c>
@@ -12541,7 +12550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>1096</v>
       </c>
@@ -12591,7 +12600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1097</v>
       </c>
@@ -12641,7 +12650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1097</v>
       </c>
@@ -12691,7 +12700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1098</v>
       </c>
@@ -12741,7 +12750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>1098</v>
       </c>
@@ -12791,7 +12800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>1099</v>
       </c>
@@ -12841,7 +12850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>1099</v>
       </c>
@@ -12891,7 +12900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>1099</v>
       </c>
@@ -12941,7 +12950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>1100</v>
       </c>
@@ -12991,7 +13000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>1100</v>
       </c>
@@ -13041,43 +13050,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>243</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R231"/>
+  <autoFilter ref="A1:R231">
+    <filterColumn colId="16">
+      <filters>
+        <filter val="last token is emoji"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>